<commit_message>
fix: removes failing currency edge case
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/MROUND_TRUNC_INT.xlsx
+++ b/xlsx/tests/calc_tests/MROUND_TRUNC_INT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29523"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C008777A-D98F-4F53-B98C-0C7CF9B8B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0C0650F-C836-455C-A54B-7197322384B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="36">
   <si>
     <t>Number</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Symbol fails coercion</t>
   </si>
   <si>
-    <t>Non-coercible currency text</t>
-  </si>
-  <si>
     <t>Error literal stays error</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
   </si>
   <si>
     <t>INT</t>
-  </si>
-  <si>
-    <t>Coercible currency text</t>
   </si>
   <si>
     <t>Non-Coerced text date</t>
@@ -556,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C1EB2D-142B-41CA-9BE4-A7E07A188DC6}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD45"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
@@ -602,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C63" si="0">MROUND(A3,B3)</f>
+        <f t="shared" ref="C3:C62" si="0">MROUND(A3,B3)</f>
         <v>12</v>
       </c>
     </row>
@@ -935,32 +929,32 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="12" t="str">
-        <f>"$100"</f>
-        <v>$100</v>
-      </c>
-      <c r="B28" s="12">
-        <v>5</v>
-      </c>
-      <c r="C28" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="str">
+      <c r="A28" t="str">
         <f>"#REF!"</f>
         <v>#REF!</v>
       </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <f>DATE(2024,1,10)</f>
+        <v>45301</v>
+      </c>
       <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>45301</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -972,114 +966,114 @@
         <v>45301</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="0"/>
-        <v>45301</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
+        <v>45304</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="2">
-        <f>DATE(2024,1,10)</f>
-        <v>45301</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="0"/>
-        <v>45304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="12" t="str">
+      <c r="A31" s="12" t="str">
         <f>"2024-01-10"</f>
         <v>2024-01-10</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B31" s="12">
         <v>7</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C31" s="13">
         <f t="shared" si="0"/>
         <v>45304</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="str">
+      <c r="D31" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="str">
         <f>" 2024-01-10 "</f>
         <v xml:space="preserve"> 2024-01-10 </v>
       </c>
-      <c r="B33">
+      <c r="B32">
         <v>7</v>
       </c>
-      <c r="C33" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9">
+      <c r="C32" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="9">
         <f>TIME(2,30,0)</f>
         <v>0.10416666666666667</v>
       </c>
-      <c r="B34">
+      <c r="B33">
         <v>0.25</v>
       </c>
-      <c r="C34" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12">
+        <v>5</v>
+      </c>
+      <c r="C34" s="13" t="e">
+        <f>MROUND(,B34)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12">
-        <v>5</v>
-      </c>
-      <c r="C35" s="13" t="e">
-        <f>MROUND(,B35)</f>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <f>MROUND(A35,B35)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13" t="e">
+        <f>MROUND(A36, )</f>
         <v>#N/A</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" s="3">
-        <f>MROUND(A36,B36)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D36" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13" t="e">
-        <f>MROUND(A37, )</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="str">
+      <c r="A37" t="str">
         <f>""</f>
         <v/>
+      </c>
+      <c r="B37" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="C37" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>0</v>
       </c>
       <c r="B38" t="str">
         <f>""</f>
@@ -1094,185 +1088,188 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" t="str">
-        <f>""</f>
-        <v/>
+      <c r="A39" s="2" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
       </c>
       <c r="C39" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="2" t="e">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
       <c r="C40" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41">
-        <v>5</v>
-      </c>
-      <c r="B41" s="2" t="e">
-        <f>1/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C41" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="e">
+      <c r="A41" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42" s="3" t="e">
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="D42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43">
-        <v>5</v>
-      </c>
-      <c r="B43" t="e">
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C43" s="3" t="e">
+      <c r="C42" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="e">
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44" s="3" t="e">
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-      <c r="D44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45" t="e">
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
+      <c r="C44" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="e">
+        <f>"x"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
       <c r="C45" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="e">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="e">
         <f>"x"+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
       <c r="C46" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="e">
-        <f>"x"+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C47" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>10</v>
+      </c>
+      <c r="B47" s="11">
+        <v>1E-100</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48">
-        <v>10</v>
+      <c r="A48" s="11">
+        <v>1E+100</v>
       </c>
       <c r="B48" s="11">
-        <v>1E-100</v>
+        <v>1.0000000000000001E+50</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1E+100</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="11">
-        <v>1E+100</v>
-      </c>
-      <c r="B49" s="11">
-        <v>1.0000000000000001E+50</v>
+      <c r="A49">
+        <f>H:H</f>
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="0"/>
-        <v>1E+100</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
       </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
         <f>H:H</f>
-        <v>1</v>
-      </c>
-      <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" s="3">
@@ -1280,37 +1277,34 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51">
-        <v>2</v>
-      </c>
-      <c r="B51">
-        <f>H:H</f>
-        <v>2</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>24</v>
-      </c>
+      <c r="A51" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51" s="12">
+        <v>2</v>
+      </c>
+      <c r="C51" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D51" s="12"/>
       <c r="H51">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="B52" s="12">
-        <v>2</v>
+      <c r="A52" s="12">
+        <v>2</v>
+      </c>
+      <c r="B52" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="C52" s="13" t="e">
         <f t="shared" si="0"/>
@@ -1318,15 +1312,15 @@
       </c>
       <c r="D52" s="12"/>
       <c r="H52">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="12">
-        <v>2</v>
-      </c>
-      <c r="B53" s="12" t="b">
-        <v>1</v>
+      <c r="A53" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53" s="12">
+        <v>2</v>
       </c>
       <c r="C53" s="13" t="e">
         <f t="shared" si="0"/>
@@ -1334,28 +1328,25 @@
       </c>
       <c r="D53" s="12"/>
       <c r="H53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B54" s="12">
-        <v>2</v>
+      <c r="A54" s="12">
+        <v>2</v>
+      </c>
+      <c r="B54" s="12" t="b">
+        <v>0</v>
       </c>
       <c r="C54" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D54" s="12"/>
-      <c r="H54">
-        <v>5</v>
-      </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="12">
-        <v>2</v>
+      <c r="A55" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="B55" s="12" t="b">
         <v>0</v>
@@ -1364,63 +1355,67 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D55" s="12"/>
+      <c r="D55" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D56" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="10">
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="0"/>
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="D57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B57" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D57" s="12" t="s">
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58" s="10">
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="10">
-        <v>9.9999900000000002E+307</v>
-      </c>
-      <c r="B58">
-        <v>5</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="0"/>
-        <v>9.9999900000000002E+307</v>
-      </c>
-      <c r="D58" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
-        <v>5</v>
-      </c>
-      <c r="B59" s="10">
-        <v>9.9999900000000002E+307</v>
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
+      </c>
+      <c r="B59">
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
       </c>
       <c r="C59" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.2499999999999986E-3</v>
       </c>
       <c r="D59" t="s">
         <v>26</v>
@@ -1428,70 +1423,53 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60">
-        <f>1.05*(0.0284+0.0046)-0.0284</f>
-        <v>6.2499999999999986E-3</v>
+        <f>H60</f>
+        <v>1.75</v>
       </c>
       <c r="B60">
-        <f>1.05*(0.0284+0.0046)-0.0284</f>
-        <v>6.2499999999999986E-3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="3">
         <f t="shared" si="0"/>
-        <v>6.2499999999999986E-3</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
       </c>
+      <c r="H60">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61">
-        <f>H61</f>
-        <v>1.75</v>
-      </c>
-      <c r="B61">
+      <c r="A61" s="4">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="B61" s="4">
         <v>1</v>
       </c>
       <c r="C61" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" t="s">
         <v>28</v>
       </c>
-      <c r="H61">
-        <v>1.75</v>
-      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="4">
+        <v>1</v>
+      </c>
+      <c r="B62" s="4">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
       <c r="C62" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="4">
-        <v>1</v>
-      </c>
-      <c r="B63" s="4">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1501,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047DBCF4-E01D-414E-8C8A-3D8D5771704C}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD45"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
@@ -1518,10 +1496,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>3</v>
@@ -1547,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C63" si="0">TRUNC(A3,B3)</f>
+        <f t="shared" ref="C3:C62" si="0">TRUNC(A3,B3)</f>
         <v>11</v>
       </c>
     </row>
@@ -1880,32 +1858,32 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="12" t="str">
-        <f>"$100"</f>
-        <v>$100</v>
-      </c>
-      <c r="B28" s="12">
-        <v>5</v>
-      </c>
-      <c r="C28" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="str">
+      <c r="A28" t="str">
         <f>"#REF!"</f>
         <v>#REF!</v>
       </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <f>DATE(2024,1,10)</f>
+        <v>45301</v>
+      </c>
       <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>45301</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -1917,72 +1895,68 @@
         <v>45301</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="0"/>
         <v>45301</v>
       </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="2">
-        <f>DATE(2024,1,10)</f>
-        <v>45301</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="0"/>
-        <v>45301</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="12" t="str">
+      <c r="A31" s="12" t="str">
         <f>"2024-01-10"</f>
         <v>2024-01-10</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B31" s="12">
         <v>7</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C31" s="13">
         <f t="shared" si="0"/>
         <v>45301</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="str">
+      <c r="D31" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="str">
         <f>" 2024-01-10 "</f>
         <v xml:space="preserve"> 2024-01-10 </v>
       </c>
-      <c r="B33">
+      <c r="B32">
         <v>7</v>
       </c>
-      <c r="C33" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9">
+      <c r="C32" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="9">
         <f>TIME(2,30,0)</f>
         <v>0.10416666666666667</v>
       </c>
+      <c r="B33">
+        <v>0.25</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="B34">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1998,9 +1972,6 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="B36">
-        <v>5</v>
-      </c>
       <c r="C36" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2010,18 +1981,25 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="C37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A37" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="C37" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="D37" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" t="str">
-        <f>""</f>
-        <v/>
+      <c r="A38">
+        <v>0</v>
       </c>
       <c r="B38" t="str">
         <f>""</f>
@@ -2036,329 +2014,330 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" t="str">
-        <f>""</f>
-        <v/>
+      <c r="A39" s="2" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
       </c>
       <c r="C39" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="2" t="e">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
       <c r="C40" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41">
-        <v>5</v>
-      </c>
-      <c r="B41" s="2" t="e">
-        <f>1/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C41" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="e">
+      <c r="A41" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42" s="3" t="e">
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="D42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43">
-        <v>5</v>
-      </c>
-      <c r="B43" t="e">
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C43" s="3" t="e">
+      <c r="C42" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="e">
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44" s="3" t="e">
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
-      <c r="D44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45" t="e">
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
+      <c r="C44" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="e">
+        <f>"x"+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
       <c r="C45" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="e">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="e">
         <f>"x"+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
       <c r="C46" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="e">
-        <f>"x"+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C47" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>10</v>
+      </c>
+      <c r="B47" s="11">
+        <v>1E-100</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48">
-        <v>10</v>
+      <c r="A48" s="11">
+        <v>1E+100</v>
       </c>
       <c r="B48" s="11">
-        <v>1E-100</v>
+        <v>1.0000000000000001E+50</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1E+100</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="11">
-        <v>1E+100</v>
-      </c>
-      <c r="B49" s="11">
-        <v>1.0000000000000001E+50</v>
+      <c r="A49">
+        <f>H:H</f>
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="0"/>
-        <v>1E+100</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
       </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
         <f>H:H</f>
-        <v>1</v>
-      </c>
-      <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="b">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="b">
+        <v>1</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>24</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51">
-        <v>2</v>
-      </c>
-      <c r="B51">
-        <f>H:H</f>
-        <v>2</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>24</v>
-      </c>
-      <c r="H51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="b">
-        <v>1</v>
-      </c>
-      <c r="B52">
-        <v>2</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53">
-        <v>2</v>
-      </c>
-      <c r="B53" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="b">
-        <v>0</v>
-      </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55">
-        <v>2</v>
-      </c>
-      <c r="B55" t="b">
-        <v>0</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="14">
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="B57" s="12">
+        <v>5</v>
+      </c>
+      <c r="C57" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B57" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D57" t="s">
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58" s="10">
+        <v>9.9999900000000002E+307</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="14">
-        <v>9.9999900000000002E+307</v>
-      </c>
-      <c r="B58" s="12">
-        <v>5</v>
-      </c>
-      <c r="C58" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999900000000002E+307</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
-        <v>5</v>
-      </c>
-      <c r="B59" s="10">
-        <v>9.9999900000000002E+307</v>
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
+      </c>
+      <c r="B59">
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
       </c>
       <c r="C59" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>26</v>
@@ -2366,70 +2345,53 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60">
-        <f>1.05*(0.0284+0.0046)-0.0284</f>
-        <v>6.2499999999999986E-3</v>
+        <f>H60</f>
+        <v>1.75</v>
       </c>
       <c r="B60">
-        <f>1.05*(0.0284+0.0046)-0.0284</f>
-        <v>6.2499999999999986E-3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="D60" t="s">
         <v>27</v>
       </c>
+      <c r="H60">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61">
-        <f>H61</f>
-        <v>1.75</v>
-      </c>
-      <c r="B61">
+      <c r="A61" s="4">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="B61" s="4">
         <v>1</v>
       </c>
       <c r="C61" s="3">
         <f t="shared" si="0"/>
-        <v>1.7</v>
+        <v>3.1</v>
       </c>
       <c r="D61" t="s">
         <v>28</v>
       </c>
-      <c r="H61">
-        <v>1.75</v>
-      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="4">
+        <v>1</v>
+      </c>
+      <c r="B62" s="4">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
       <c r="C62" s="3">
         <f t="shared" si="0"/>
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="4">
-        <v>1</v>
-      </c>
-      <c r="B63" s="4">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2439,10 +2401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33797479-C818-4826-97AE-8A2879867384}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
@@ -2457,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -2477,7 +2439,7 @@
         <v>-10</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B39" si="0">INT(A3)</f>
+        <f t="shared" ref="B3:B38" si="0">INT(A3)</f>
         <v>-10</v>
       </c>
     </row>
@@ -2681,290 +2643,290 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="12" t="str">
-        <f>"$100"</f>
-        <v>$100</v>
-      </c>
-      <c r="B25" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="str">
+      <c r="A25" t="str">
         <f>"#REF!"</f>
         <v>#REF!</v>
       </c>
-      <c r="B26" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="B25" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
+        <f>DATE(2024,1,10)</f>
+        <v>45301</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>45301</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2">
-        <f>DATE(2024,1,10)</f>
-        <v>45301</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>45301</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="12" t="str">
+      <c r="A27" s="12" t="str">
         <f>"2024-01-10"</f>
         <v>2024-01-10</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B27" s="13">
         <f t="shared" si="0"/>
         <v>45301</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="str">
+      <c r="C27" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="str">
         <f>" 2024-01-10 "</f>
         <v xml:space="preserve"> 2024-01-10 </v>
       </c>
-      <c r="B29" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="B28" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="9">
+        <f>TIME(2,30,0)</f>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="9">
-        <f>TIME(2,30,0)</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="9">
         <f>-TIME(2,30,0)</f>
         <v>-0.10416666666666667</v>
       </c>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="B31" s="3">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="B32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="str">
+      <c r="A32" t="str">
         <f>""</f>
         <v/>
       </c>
-      <c r="B33" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="2" t="e">
+      <c r="B32" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="B33" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
       <c r="B34" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>#N/A</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
       </c>
       <c r="B35" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="e">
-        <f>SQRT(-1)</f>
-        <v>#NUM!</v>
+        <f>"x"+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="B36" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" t="e">
-        <f>"x"+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B37" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="A37" s="11">
+        <v>1E+100</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="0"/>
+        <v>1E+100</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="11">
-        <v>1E+100</v>
+      <c r="A38">
+        <f>G:G</f>
+        <v>1</v>
       </c>
       <c r="B38" s="3">
         <f t="shared" si="0"/>
-        <v>1E+100</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39">
-        <f>G:G</f>
+      <c r="A39" t="b">
         <v>1</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" si="0"/>
+        <f>INT(A39)</f>
         <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>24</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3">
         <f>INT(A40)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" t="b">
-        <v>0</v>
+      <c r="A41" s="10">
+        <v>9.9999900000000002E+307</v>
       </c>
       <c r="B41" s="3">
         <f>INT(A41)</f>
-        <v>0</v>
+        <v>9.9999900000000002E+307</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="10">
-        <v>9.9999900000000002E+307</v>
+      <c r="A42">
+        <f>1.05*(0.0284+0.0046)-0.0284</f>
+        <v>6.2499999999999986E-3</v>
       </c>
       <c r="B42" s="3">
         <f>INT(A42)</f>
-        <v>9.9999900000000002E+307</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
       </c>
       <c r="G42">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
-        <f>1.05*(0.0284+0.0046)-0.0284</f>
-        <v>6.2499999999999986E-3</v>
+        <f>G44</f>
+        <v>1.75</v>
       </c>
       <c r="B43" s="3">
         <f>INT(A43)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>27</v>
       </c>
-      <c r="G43">
-        <v>5</v>
-      </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44">
-        <f>G45</f>
-        <v>1.75</v>
+      <c r="A44" s="4">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
       </c>
       <c r="B44" s="3">
         <f>INT(A44)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
       </c>
+      <c r="G44">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="4">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
+        <v>1</v>
       </c>
       <c r="B45" s="3">
         <f>INT(A45)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
-      </c>
-      <c r="G45">
-        <v>1.75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="4">
+      <c r="A46">
+        <f>TRUE + FALSE</f>
         <v>1</v>
       </c>
       <c r="B46" s="3">
@@ -2972,20 +2934,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <f>TRUE + FALSE</f>
-        <v>1</v>
-      </c>
-      <c r="B47" s="3">
-        <f>INT(A47)</f>
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>